<commit_message>
Item & Perk Update
</commit_message>
<xml_diff>
--- a/Documentation/Testing/Item Testing Tables.xlsx
+++ b/Documentation/Testing/Item Testing Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Rifle" sheetId="1" r:id="rId1"/>
@@ -702,8 +702,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="279">
+  <cellStyleXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1181,7 +1185,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="279">
+  <cellStyles count="283">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1321,6 +1325,8 @@
     <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1460,6 +1466,8 @@
     <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3752,7 +3760,7 @@
   <dimension ref="B2:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>